<commit_message>
Add target and sales sigh in columns name
</commit_message>
<xml_diff>
--- a/new_testdata2.xlsx
+++ b/new_testdata2.xlsx
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,10 +430,10 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.1244045781371552</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.9826406370400775</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -442,18 +442,18 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>0.1735427119226257</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>0.4191043763702654</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <v>0.03708291682538347</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>0.0427953287245139</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -480,10 +480,10 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>0.2644460372154296</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1.35402952365778</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -512,24 +512,24 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>32.72627536024244</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>33.06626842723345</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>0.385638222623379</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>0.9778791529581891</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>4.105514763122162</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>8.023940643412423</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -556,10 +556,10 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>2.97488563686306</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1.289494588390176</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -582,10 +582,10 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>5.308046678850264</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>5.601476461478329</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -594,10 +594,10 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>5.164777939627022</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>6.98482447092498</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -608,10 +608,10 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0.7571449731147208</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0.9625724567901733</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -632,10 +632,10 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>7.272266023424316</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>4.513431745525934</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -646,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0.8999165948697907</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -670,10 +670,10 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>16.96767760100764</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>16.33341654641623</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -702,16 +702,16 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>8.642591779975234</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>7.377389821827624</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>27.68296356525348</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>25.14514447360845</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -722,10 +722,10 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>2.033397566551004</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1.286820936254986</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -746,10 +746,10 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>39.11380226206305</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>42.98267512214798</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -766,10 +766,10 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0.1471096748118517</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>0.09947366426078569</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -778,10 +778,10 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>0.6226210791404801</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1.865849732498522</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -816,16 +816,16 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>1.639316513031779</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>5.038613462025728</v>
       </c>
       <c r="K12">
-        <v>4.223223794664877</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>4.511104823957952</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -836,10 +836,10 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>2.790513681756166</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>4.329706352573461</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -854,10 +854,10 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>4.571323494546493</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1.968274023369803</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -892,10 +892,10 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>3.003927808521584</v>
+        <v>8.27556144976719</v>
       </c>
       <c r="J14">
-        <v>1.968274023369803</v>
+        <v>8.916870955805498</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -912,10 +912,10 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>7.709909981214076</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>6.176984643614591</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -930,10 +930,10 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>8.511835740741928</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>7.377389821827624</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -956,10 +956,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>97.07397628439421</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>96.42837207847253</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -968,10 +968,10 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>11.15996241563942</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>8.109497208726548</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -982,10 +982,10 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17">
-        <v>0.3337307048134242</v>
+        <v>0</v>
       </c>
       <c r="B17">
-        <v>0.3438750152126752</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1006,10 +1006,10 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>20.64977164777899</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>14.95888257761051</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -1020,10 +1020,10 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18">
-        <v>0.1716303899124969</v>
+        <v>0</v>
       </c>
       <c r="B18">
-        <v>0.1570797786340439</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1044,10 +1044,10 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>21.87112668867043</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>18.69835379090232</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -1070,10 +1070,10 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0.1604477056249856</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0.4223544078636697</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1082,10 +1082,10 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>22.69848097068329</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>33.06626842723345</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -1114,10 +1114,10 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>0.4222366318254477</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>0.9923481590328036</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1126,10 +1126,10 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <v>1.0106539367926</v>
+        <v>0</v>
       </c>
       <c r="L20">
-        <v>0.977375002630857</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1146,16 +1146,16 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0.7125492390202296</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0.8738084083154152</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>0.7037746599251754</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>2.366312778236024</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1190,10 +1190,10 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>0.932992847552697</v>
+        <v>4.644809487030747</v>
       </c>
       <c r="H22">
-        <v>0.9825969427612281</v>
+        <v>3.549390253434932</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1216,10 +1216,10 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>15.87253899987758</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>16.29876543376681</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1228,10 +1228,10 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>6.896991667266719</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>5.657065081836256</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1254,10 +1254,10 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>28.65000178822846</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>20.01772320894699</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1266,10 +1266,10 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>87.33218755395191</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>87.43488372745999</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -1292,16 +1292,16 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>0.2595942112341648</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>0.03809864712110639</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>0.3567609425795917</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1336,10 +1336,10 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.08890249003626782</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.4252183902787009</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1348,10 +1348,10 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>7.509719343627427</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>8.916870955805498</v>
+        <v>0</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -1374,10 +1374,10 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>0.09524238273750128</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>0.4435232593774707</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1392,10 +1392,10 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <v>26.39397507731725</v>
+        <v>0</v>
       </c>
       <c r="L27">
-        <v>25.13218077274742</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1412,10 +1412,10 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>0.1600007656997999</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>0.5242184089857995</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1430,10 +1430,10 @@
         <v>0</v>
       </c>
       <c r="K28">
-        <v>1.272324952445037</v>
+        <v>0</v>
       </c>
       <c r="L28">
-        <v>1.288829783217816</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1444,16 +1444,16 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>0.6705885591817142</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>0.6818435200903088</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>0.3714491042349933</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>0.2882930768633495</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1488,10 +1488,10 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>0.9870412508485481</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>0.8797336972882004</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1506,18 +1506,18 @@
         <v>0</v>
       </c>
       <c r="K30">
-        <v>2.631393287445038</v>
+        <v>0</v>
       </c>
       <c r="L30">
-        <v>1.353331447187386</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31">
-        <v>15.93383739416571</v>
+        <v>0</v>
       </c>
       <c r="B31">
-        <v>8.972143512686515</v>
+        <v>0</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1526,10 +1526,10 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>98.25926535932177</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>97.08225222462688</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1558,10 +1558,10 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>0.2992388439095395</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>0.9625724567901734</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1570,10 +1570,10 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <v>3.296721320634614</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>3.51451250243754</v>
+        <v>0</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -1596,16 +1596,16 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>0.4103827450376586</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0.3055816778286164</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>0.4405359877905531</v>
+        <v>0</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1628,16 +1628,16 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34">
-        <v>2.913435656065458</v>
+        <v>0</v>
       </c>
       <c r="B34">
-        <v>3.445121836173185</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>0.7694419851931689</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>0.6818435200903089</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1672,10 +1672,10 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1.346523474088045</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1.286820936254987</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1696,24 +1696,24 @@
         <v>0</v>
       </c>
       <c r="K35">
-        <v>7.534757329001502</v>
+        <v>0</v>
       </c>
       <c r="L35">
-        <v>6.981223410883233</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36">
-        <v>29.82378251065734</v>
+        <v>0</v>
       </c>
       <c r="B36">
-        <v>28.84365004280024</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1.795444468680544</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>1.143891696724708</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1748,10 +1748,10 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>0.9518454411919376</v>
+        <v>2.564806617310563</v>
       </c>
       <c r="D37">
-        <v>0.886435992542878</v>
+        <v>4.329706352573461</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1780,16 +1780,16 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38">
-        <v>4.580328172648608</v>
+        <v>0</v>
       </c>
       <c r="B38">
-        <v>3.269150509106485</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>3.590888937361088</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>0.8864359925428781</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1824,10 +1824,10 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>8.771985349990661</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>6.176984643614592</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1842,10 +1842,10 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <v>16.53455750219723</v>
+        <v>0</v>
       </c>
       <c r="J39">
-        <v>18.69835379090232</v>
+        <v>0</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -1862,10 +1862,10 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>8.848976309925538</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>28.5972924181177</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1880,10 +1880,10 @@
         <v>0</v>
       </c>
       <c r="I40">
-        <v>10.6873025181645</v>
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>8.109497208726548</v>
+        <v>0</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -1900,10 +1900,10 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>10.62338384421605</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>8.75099222169267</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1924,10 +1924,10 @@
         <v>0</v>
       </c>
       <c r="K41">
-        <v>-0.05414389480339585</v>
+        <v>0</v>
       </c>
       <c r="L41">
-        <v>0.05155548370237659</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -1938,16 +1938,16 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>14.42618183062388</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>16.29876543376681</v>
       </c>
       <c r="E42">
-        <v>0.4620209084231675</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>0.5206876296514746</v>
+        <v>0</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -1976,16 +1976,16 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>16.92847641898799</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>10.86697111888473</v>
       </c>
       <c r="E43">
-        <v>0.09167042693329973</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>0.05747788547295332</v>
+        <v>0</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -2014,10 +2014,10 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <v>2.033487988000958</v>
+        <v>29.62426917467527</v>
       </c>
       <c r="D44">
-        <v>1.143891696724708</v>
+        <v>20.01772320894699</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -2046,10 +2046,10 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45">
-        <v>0</v>
+        <v>0.2413350402456683</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>0.3675400741575188</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -2058,10 +2058,10 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>0.09167314454348985</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>0.309940988371858</v>
+        <v>0</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -2084,10 +2084,10 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46">
-        <v>0.06356869551688762</v>
+        <v>0.3619971947444142</v>
       </c>
       <c r="B46">
-        <v>0.3668054530397108</v>
+        <v>0.3445637123025586</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -2122,10 +2122,10 @@
     </row>
     <row r="47" spans="1:12">
       <c r="A47">
-        <v>0</v>
+        <v>5.140664932818899</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>3.275697813628217</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -2146,10 +2146,10 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>17.44386148457271</v>
+        <v>0</v>
       </c>
       <c r="J47">
-        <v>14.95888257761051</v>
+        <v>0</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -2160,16 +2160,16 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48">
-        <v>0</v>
+        <v>6.033429662382592</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>8.04001062327734</v>
       </c>
       <c r="C48">
-        <v>9.767542420213218</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>8.750992221692668</v>
+        <v>0</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -2198,10 +2198,10 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49">
-        <v>0</v>
+        <v>6.083383622645102</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>3.452021567988243</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2228,24 +2228,24 @@
         <v>0</v>
       </c>
       <c r="K49">
-        <v>15.44819932127534</v>
+        <v>0</v>
       </c>
       <c r="L49">
-        <v>16.3249957745106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50">
-        <v>0</v>
+        <v>15.96549495923762</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>8.990112509716967</v>
       </c>
       <c r="C50">
-        <v>13.67196179166602</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>10.86697111888473</v>
+        <v>0</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -2274,10 +2274,10 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51">
-        <v>0</v>
+        <v>29.36190764247839</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>28.90141678061865</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -2304,18 +2304,18 @@
         <v>0</v>
       </c>
       <c r="K51">
-        <v>0.3925432373246199</v>
+        <v>0</v>
       </c>
       <c r="L51">
-        <v>0.41888830508181</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:12">
       <c r="A52">
-        <v>0</v>
+        <v>36.81178694544733</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>46.62863691831051</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2330,10 +2330,10 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>2.280801307318473</v>
+        <v>0</v>
       </c>
       <c r="H52">
-        <v>2.343060427277605</v>
+        <v>0</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -2346,348 +2346,6 @@
       </c>
       <c r="L52">
         <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12">
-      <c r="A53">
-        <v>0</v>
-      </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>0.4278333722313938</v>
-      </c>
-      <c r="F53">
-        <v>0.206639576334245</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53">
-        <v>0</v>
-      </c>
-      <c r="J53">
-        <v>0</v>
-      </c>
-      <c r="K53">
-        <v>0</v>
-      </c>
-      <c r="L53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
-      <c r="A54">
-        <v>0</v>
-      </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <v>0</v>
-      </c>
-      <c r="I54">
-        <v>3.035446869064472</v>
-      </c>
-      <c r="J54">
-        <v>5.038613462025728</v>
-      </c>
-      <c r="K54">
-        <v>0</v>
-      </c>
-      <c r="L54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12">
-      <c r="A55">
-        <v>42.03708879627251</v>
-      </c>
-      <c r="B55">
-        <v>46.5354378802102</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="I55">
-        <v>0</v>
-      </c>
-      <c r="J55">
-        <v>0</v>
-      </c>
-      <c r="K55">
-        <v>0</v>
-      </c>
-      <c r="L55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12">
-      <c r="A56">
-        <v>0</v>
-      </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <v>0.4163173336344053</v>
-      </c>
-      <c r="J56">
-        <v>1.865849732498522</v>
-      </c>
-      <c r="K56">
-        <v>0</v>
-      </c>
-      <c r="L56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12">
-      <c r="A57">
-        <v>0</v>
-      </c>
-      <c r="B57">
-        <v>0</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>0.1100142957166441</v>
-      </c>
-      <c r="F57">
-        <v>0.3543580430595399</v>
-      </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="I57">
-        <v>0</v>
-      </c>
-      <c r="J57">
-        <v>0</v>
-      </c>
-      <c r="K57">
-        <v>0</v>
-      </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
-      <c r="A58">
-        <v>0</v>
-      </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58">
-        <v>0</v>
-      </c>
-      <c r="G58">
-        <v>88.0570332675068</v>
-      </c>
-      <c r="H58">
-        <v>86.57571302900521</v>
-      </c>
-      <c r="I58">
-        <v>0</v>
-      </c>
-      <c r="J58">
-        <v>0</v>
-      </c>
-      <c r="K58">
-        <v>0</v>
-      </c>
-      <c r="L58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12">
-      <c r="A59">
-        <v>0</v>
-      </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
-      <c r="C59">
-        <v>0</v>
-      </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59">
-        <v>0.4171232704721108</v>
-      </c>
-      <c r="F59">
-        <v>0.2863513304069681</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59">
-        <v>0</v>
-      </c>
-      <c r="J59">
-        <v>0</v>
-      </c>
-      <c r="K59">
-        <v>0</v>
-      </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12">
-      <c r="A60">
-        <v>0</v>
-      </c>
-      <c r="B60">
-        <v>0</v>
-      </c>
-      <c r="C60">
-        <v>13.93155600290018</v>
-      </c>
-      <c r="D60">
-        <v>28.5972924181177</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
-      <c r="G60">
-        <v>0</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
-      <c r="A61">
-        <v>0</v>
-      </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="I61">
-        <v>0</v>
-      </c>
-      <c r="J61">
-        <v>0</v>
-      </c>
-      <c r="K61">
-        <v>41.14707295853713</v>
-      </c>
-      <c r="L61">
-        <v>42.96051519608054</v>
       </c>
     </row>
   </sheetData>

</xml_diff>